<commit_message>
Add row with email and birthyear
</commit_message>
<xml_diff>
--- a/BeerTaste.Console/BeerTaste.xlsx
+++ b/BeerTaste.Console/BeerTaste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\s\aklefdal\beertaste\BeerTaste.Console\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A236709-7D42-4FD6-8DE6-A9E83D1837DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409C950B-79B5-49F0-991C-6A3A1FD8D3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{BC7F52BA-51F1-4635-A5AB-EB1BCFC6D5AD}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="38700" windowHeight="15225" activeTab="2" xr2:uid="{BC7F52BA-51F1-4635-A5AB-EB1BCFC6D5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Beers" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Nr</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Score 0 - 10</t>
+  </si>
+  <si>
+    <t>Epost:</t>
+  </si>
+  <si>
+    <t>Fødselsår:</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +163,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -272,7 +285,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -614,18 +635,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -654,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -693,16 +714,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6295EB-4F56-4FE0-8965-9FF25FB9A6DB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -713,7 +736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -734,59 +757,78 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" customWidth="1"/>
-    <col min="4" max="4" width="29.54296875" customWidth="1"/>
-    <col min="5" max="5" width="26.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="47.5" x14ac:dyDescent="1.1000000000000001">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A1" s="19" t="s">
         <v>19</v>
       </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.4">
+      <c r="A2" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8"/>
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>